<commit_message>
5 year data testing
</commit_message>
<xml_diff>
--- a/optimization_annual_summary.xlsx
+++ b/optimization_annual_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,50 +451,55 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Battery total Capacity (MWh)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Per Unit Cost (INR/MWh)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Final Cost (INR)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total Cost (INR)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Annual Demand Offset (%)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Annual Demand Met (MWh)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Annual Curtailment (%)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Annual Generation (MWh)</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Annual Demand (MWh)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>OA Cost (INR)</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Objective Aggregate Cost (INR)</t>
         </is>
@@ -502,43 +507,46 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>441.1212376442786</v>
+        <v>446.5698322765596</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>223.5117637822168</v>
+        <v>250</v>
       </c>
       <c r="D2" t="n">
-        <v>20999.20811564427</v>
+        <v>2500</v>
       </c>
       <c r="E2" t="n">
-        <v>21999.20811564427</v>
+        <v>4459.25831949529</v>
       </c>
       <c r="F2" t="n">
-        <v>20694719597.96744</v>
+        <v>5459.25831949529</v>
       </c>
       <c r="G2" t="n">
-        <v>44.99999999999999</v>
+        <v>21972995369.31326</v>
       </c>
       <c r="H2" t="n">
-        <v>985500.0000000003</v>
+        <v>45.00000000000043</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>4927500.000000047</v>
       </c>
       <c r="J2" t="n">
-        <v>1005990.564358946</v>
+        <v>3.364582101824124e-12</v>
       </c>
       <c r="K2" t="n">
-        <v>2190000</v>
+        <v>5041414.416467906</v>
       </c>
       <c r="L2" t="n">
+        <v>10950000</v>
+      </c>
+      <c r="M2" t="n">
         <v>1000</v>
       </c>
-      <c r="M2" t="n">
-        <v>20661877586.59878</v>
+      <c r="N2" t="n">
+        <v>21587498190.05507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>